<commit_message>
Completed lnCVR and now am beginning meta-regression on the traits
</commit_message>
<xml_diff>
--- a/data/Overall_effects_not_split.xlsx
+++ b/data/Overall_effects_not_split.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamanw\Dropbox\Meta Analysis Project\Extraction\Transgenerational Meta-Analysis\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C36DED-4C63-4442-9CDF-0BA3653D09C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11CB568-FF12-4D07-AFC8-E77B82C03D00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Experiment_Type</t>
   </si>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t>F0 Male</t>
-  </si>
-  <si>
-    <t>Mice</t>
-  </si>
-  <si>
-    <t>Rats</t>
   </si>
   <si>
     <t>Grand Offspring (Both)</t>
@@ -399,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:E9"/>
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,13 +497,13 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>0.22140000000000001</v>
+        <v>0.48709999999999998</v>
       </c>
       <c r="D5">
-        <v>1.7999999999999999E-2</v>
+        <v>0.17430000000000001</v>
       </c>
       <c r="E5">
-        <v>0.42480000000000001</v>
+        <v>0.79979999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -520,13 +514,13 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>-4.1099999999999998E-2</v>
+        <v>-0.34189999999999998</v>
       </c>
       <c r="D6">
-        <v>-0.30580000000000002</v>
+        <v>-0.63029999999999997</v>
       </c>
       <c r="E6">
-        <v>0.2235</v>
+        <v>-5.3499999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -537,46 +531,12 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>0.48709999999999998</v>
+        <v>-0.32500000000000001</v>
       </c>
       <c r="D7">
-        <v>0.17430000000000001</v>
+        <v>-0.61439999999999995</v>
       </c>
       <c r="E7">
-        <v>0.79979999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>-0.34189999999999998</v>
-      </c>
-      <c r="D8">
-        <v>-0.63029999999999997</v>
-      </c>
-      <c r="E8">
-        <v>-5.3499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>-0.32500000000000001</v>
-      </c>
-      <c r="D9">
-        <v>-0.61439999999999995</v>
-      </c>
-      <c r="E9">
         <v>-3.5499999999999997E-2</v>
       </c>
     </row>

</xml_diff>